<commit_message>
added cuq violin plot
</commit_message>
<xml_diff>
--- a/res/user_data/questionare.xlsx
+++ b/res/user_data/questionare.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<x:sst xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="65">
   <x:si>
     <x:t xml:space="preserve">ID</x:t>
   </x:si>
@@ -200,6 +200,27 @@
   </x:si>
   <x:si>
     <x:t xml:space="preserve">28</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">9</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">26</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">3</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">60</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">7</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">8</x:t>
+  </x:si>
+  <x:si>
+    <x:t xml:space="preserve">27</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -296,8 +317,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AQ5" insertRow="1" totalsRowShown="0">
-  <x:autoFilter ref="A1:AQ5"/>
+<x:table xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AQ10" insertRow="1" totalsRowShown="0">
+  <x:autoFilter ref="A1:AQ10"/>
   <x:tableColumns count="43">
     <x:tableColumn id="1" uniqueName="1" name="ID" dataDxfId="0"/>
     <x:tableColumn id="2" uniqueName="2" name="Start time" dataDxfId="3"/>
@@ -1336,11 +1357,646 @@
         <x:v>51</x:v>
       </x:c>
     </x:row>
+    <x:row r="6" hidden="0">
+      <x:c r="A6">
+        <x:v>8</x:v>
+      </x:c>
+      <x:c r="B6" s="2">
+        <x:v>45224.7830787037</x:v>
+      </x:c>
+      <x:c r="C6" s="2">
+        <x:v>45224.7936458333</x:v>
+      </x:c>
+      <x:c r="D6" s="10" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="E6" s="10" t="s"/>
+      <x:c r="F6" s="2"/>
+      <x:c r="G6" s="10" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="H6" s="7" t="s">
+        <x:v>58</x:v>
+      </x:c>
+      <x:c r="I6" s="7" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="J6" s="10" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="K6" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="L6" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="M6" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="N6" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="O6" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="P6" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="Q6" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="R6" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="S6" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="T6" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="U6" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="V6" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="W6" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="X6" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="Y6" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="Z6" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AA6" s="10" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="AB6" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AC6" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AD6" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AE6" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AF6" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AG6" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AH6" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AI6" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AJ6" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AK6" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AL6" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AM6" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AN6" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AO6" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AP6" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AQ6" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" hidden="0">
+      <x:c r="A7">
+        <x:v>9</x:v>
+      </x:c>
+      <x:c r="B7" s="2">
+        <x:v>45224.8342476852</x:v>
+      </x:c>
+      <x:c r="C7" s="2">
+        <x:v>45224.8468171296</x:v>
+      </x:c>
+      <x:c r="D7" s="10" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="E7" s="10" t="s"/>
+      <x:c r="F7" s="2"/>
+      <x:c r="G7" s="10" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="H7" s="7" t="s">
+        <x:v>60</x:v>
+      </x:c>
+      <x:c r="I7" s="7" t="s">
+        <x:v>61</x:v>
+      </x:c>
+      <x:c r="J7" s="10" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="K7" s="10" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="L7" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="M7" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="N7" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="O7" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="P7" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="Q7" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="R7" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="S7" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="T7" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="U7" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="V7" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="W7" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="X7" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="Y7" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="Z7" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AA7" s="10" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="AB7" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AC7" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AD7" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AE7" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AF7" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AG7" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AH7" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AI7" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AJ7" s="10" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="AK7" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AL7" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AM7" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AN7" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AO7" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AP7" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AQ7" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" hidden="0">
+      <x:c r="A8">
+        <x:v>10</x:v>
+      </x:c>
+      <x:c r="B8" s="2">
+        <x:v>45224.9413657407</x:v>
+      </x:c>
+      <x:c r="C8" s="2">
+        <x:v>45224.9657638889</x:v>
+      </x:c>
+      <x:c r="D8" s="10" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="E8" s="10" t="s"/>
+      <x:c r="F8" s="2"/>
+      <x:c r="G8" s="10" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="H8" s="7" t="s">
+        <x:v>62</x:v>
+      </x:c>
+      <x:c r="I8" s="7" t="s">
+        <x:v>59</x:v>
+      </x:c>
+      <x:c r="J8" s="10" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="K8" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="L8" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="M8" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="N8" s="10" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="O8" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="P8" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="Q8" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="R8" s="10" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="S8" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="T8" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="U8" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="V8" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="W8" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="X8" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="Y8" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="Z8" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AA8" s="10" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="AB8" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AC8" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AD8" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AE8" s="10" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="AF8" s="10" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="AG8" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AH8" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AI8" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AJ8" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AK8" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AL8" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AM8" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AN8" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AO8" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AP8" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AQ8" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" hidden="0">
+      <x:c r="A9">
+        <x:v>11</x:v>
+      </x:c>
+      <x:c r="B9" s="2">
+        <x:v>45224.7881018519</x:v>
+      </x:c>
+      <x:c r="C9" s="2">
+        <x:v>45224.9814814815</x:v>
+      </x:c>
+      <x:c r="D9" s="10" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="E9" s="10" t="s"/>
+      <x:c r="F9" s="2"/>
+      <x:c r="G9" s="10" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="H9" s="7" t="s">
+        <x:v>63</x:v>
+      </x:c>
+      <x:c r="I9" s="7" t="s">
+        <x:v>64</x:v>
+      </x:c>
+      <x:c r="J9" s="10" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="K9" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="L9" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="M9" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="N9" s="10" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="O9" s="10" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="P9" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="Q9" s="10" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="R9" s="10" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="S9" s="10" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="T9" s="10" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="U9" s="10" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="V9" s="10" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="W9" s="10" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="X9" s="10" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="Y9" s="10" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="Z9" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AA9" s="10" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="AB9" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AC9" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AD9" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AE9" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AF9" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AG9" s="10" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="AH9" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AI9" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AJ9" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AK9" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AL9" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AM9" s="10" t="s">
+        <x:v>50</x:v>
+      </x:c>
+      <x:c r="AN9" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AO9" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AP9" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AQ9" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" hidden="0">
+      <x:c r="A10">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="B10" s="2">
+        <x:v>45225.018275463</x:v>
+      </x:c>
+      <x:c r="C10" s="2">
+        <x:v>45225.1474305556</x:v>
+      </x:c>
+      <x:c r="D10" s="10" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="E10" s="10" t="s"/>
+      <x:c r="F10" s="2"/>
+      <x:c r="G10" s="10" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="H10" s="7" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="I10" s="7" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="J10" s="10" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="K10" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="L10" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="M10" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="N10" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="O10" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="P10" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="Q10" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="R10" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="S10" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="T10" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="U10" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="V10" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="W10" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="X10" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="Y10" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="Z10" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AA10" s="10" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="AB10" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AC10" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AD10" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AE10" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AF10" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AG10" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AH10" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AI10" s="10" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="AJ10" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AK10" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AL10" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AM10" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="AN10" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AO10" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AP10" s="10" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="AQ10" s="10" t="s">
+        <x:v>48</x:v>
+      </x:c>
+    </x:row>
   </x:sheetData>
   <x:pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <x:pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <x:tableParts count="1">
-    <x:tablePart r:id="R3074dc34b9544775"/>
+    <x:tablePart r:id="R2cb2a6f052224a73"/>
   </x:tableParts>
 </x:worksheet>
 </file>
</xml_diff>